<commit_message>
Rerunning Marmot + results
</commit_message>
<xml_diff>
--- a/data/results/marmot_XPOS.xlsx
+++ b/data/results/marmot_XPOS.xlsx
@@ -1196,7 +1196,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>brev:npun</t>
+          <t>brev:pun</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -5396,7 +5396,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>part</t>
+          <t>comp</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
@@ -10796,7 +10796,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>ppron3:sg:loc:m1:ter:akc:npraep</t>
+          <t>ppron3:sg:gen:m1:ter:akc:npraep</t>
         </is>
       </c>
       <c r="E415" t="inlineStr">
@@ -19446,7 +19446,7 @@
       </c>
       <c r="D761" t="inlineStr">
         <is>
-          <t>praet:pl:n:imperf</t>
+          <t>praet:pl:f:imperf</t>
         </is>
       </c>
       <c r="E761" t="inlineStr">
@@ -28446,7 +28446,7 @@
       </c>
       <c r="D1121" t="inlineStr">
         <is>
-          <t>subst:sg:gen:n:ncol</t>
+          <t>adj:sg:gen:n:pos</t>
         </is>
       </c>
       <c r="E1121" t="inlineStr">
@@ -29746,7 +29746,7 @@
       </c>
       <c r="D1173" t="inlineStr">
         <is>
-          <t>inf:perf</t>
+          <t>inf:imperf</t>
         </is>
       </c>
       <c r="E1173" t="inlineStr">
@@ -30321,7 +30321,7 @@
       </c>
       <c r="D1196" t="inlineStr">
         <is>
-          <t>subst:sg:gen:f</t>
+          <t>subst:sg:acc:f</t>
         </is>
       </c>
       <c r="E1196" t="inlineStr">
@@ -45971,7 +45971,7 @@
       </c>
       <c r="D1822" t="inlineStr">
         <is>
-          <t>subst:sg:gen:f</t>
+          <t>adj:sg:gen:f:pos</t>
         </is>
       </c>
       <c r="E1822" t="inlineStr">
@@ -69646,7 +69646,7 @@
       </c>
       <c r="D2769" t="inlineStr">
         <is>
-          <t>subst:sg:loc:m3</t>
+          <t>subst:sg:loc:m1</t>
         </is>
       </c>
       <c r="E2769" t="inlineStr">

</xml_diff>